<commit_message>
Fixed colouring on cell in Excel version
</commit_message>
<xml_diff>
--- a/ExcelVersion.xlsx
+++ b/ExcelVersion.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEM\Projects\flatroster\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEM\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B590081A-2F4F-4459-A491-9D20E7C8C1BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9BAEBC-33C3-4145-A909-3207A4D3A23D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{83C82FFB-4246-490B-BD93-016621CF92AA}"/>
   </bookViews>
@@ -132,7 +132,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,12 +148,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF9966"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -176,13 +170,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,7 +507,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,19 +548,19 @@
         <v>14</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="5"/>
+      <c r="C2" s="4"/>
       <c r="D2" s="1"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="5"/>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="1"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="5"/>
+      <c r="E3" s="4"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
@@ -576,9 +569,9 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="5"/>
+      <c r="D4" s="4"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="4"/>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
@@ -607,13 +600,13 @@
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="1"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="5"/>
+      <c r="E6" s="4"/>
       <c r="F6" s="1"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="5"/>
+      <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
@@ -621,10 +614,10 @@
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="5"/>
+      <c r="D7" s="4"/>
       <c r="E7" s="1"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="5"/>
+      <c r="G7" s="4"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
@@ -632,10 +625,10 @@
         <v>16</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="5"/>
+      <c r="C8" s="4"/>
       <c r="D8" s="1"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="5"/>
+      <c r="F8" s="4"/>
       <c r="G8" s="1"/>
       <c r="H8" s="2"/>
     </row>
@@ -695,7 +688,7 @@
       <c r="B20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="1" t="s">

</xml_diff>